<commit_message>
Update on more requirements
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
EDA upto June 11
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>553.9339164698035</v>
+        <v>536.8469228506967</v>
       </c>
       <c r="D2" t="n">
-        <v>136.0796753216788</v>
+        <v>129.7761258031</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
       </c>
       <c r="F2" t="n">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="G2" t="n">
-        <v>513</v>
+        <v>490</v>
       </c>
       <c r="H2" t="n">
-        <v>625</v>
+        <v>594</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.54371199562761</v>
+        <v>36.37627465722989</v>
       </c>
       <c r="D3" t="n">
-        <v>6.49341519441723</v>
+        <v>6.672834355817785</v>
       </c>
       <c r="E3" t="n">
-        <v>13.99</v>
+        <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.81</v>
+        <v>31.37</v>
       </c>
       <c r="G3" t="n">
-        <v>37.81</v>
+        <v>36.49</v>
       </c>
       <c r="H3" t="n">
-        <v>41.51</v>
+        <v>40.78</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.98216252087201</v>
+        <v>1.922306955007867</v>
       </c>
       <c r="D4" t="n">
-        <v>2.542316588933395</v>
+        <v>2.60020301288987</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="G4" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
       <c r="H4" t="n">
-        <v>2.41</v>
+        <v>2.33</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.3209024386936</v>
+        <v>322.7852664719634</v>
       </c>
       <c r="D5" t="n">
-        <v>10.80527007418962</v>
+        <v>9.604742530486975</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.54</v>
+        <v>317.24</v>
       </c>
       <c r="G5" t="n">
-        <v>324.78</v>
+        <v>323.4</v>
       </c>
       <c r="H5" t="n">
-        <v>331.49</v>
+        <v>329.81</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21.20733341915513</v>
+        <v>22.16748994820075</v>
       </c>
       <c r="D6" t="n">
-        <v>2.579251734899544</v>
+        <v>2.911911700136196</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>19.73</v>
+        <v>20.31</v>
       </c>
       <c r="G6" t="n">
-        <v>21.17</v>
+        <v>22.08</v>
       </c>
       <c r="H6" t="n">
-        <v>22.53</v>
+        <v>23.97</v>
       </c>
       <c r="I6" t="n">
-        <v>40.24</v>
+        <v>43.95</v>
       </c>
     </row>
     <row r="7">
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.90280080160562</v>
+        <v>-76.7367893705309</v>
       </c>
       <c r="D7" t="n">
-        <v>22.89926493012658</v>
+        <v>22.80897747747082</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,7 +669,7 @@
         <v>-93</v>
       </c>
       <c r="G7" t="n">
-        <v>-73</v>
+        <v>-74</v>
       </c>
       <c r="H7" t="n">
         <v>-60</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.419475878633727</v>
+        <v>7.415246339073944</v>
       </c>
       <c r="D8" t="n">
-        <v>7.098372356541219</v>
+        <v>7.114583036411164</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -708,7 +708,7 @@
         <v>11.2</v>
       </c>
       <c r="I8" t="n">
-        <v>19</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322680892004572</v>
+        <v>9.322031633382492</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685704350766166</v>
+        <v>1.685562417434868</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8301139623015</v>
+        <v>867.8302641267222</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461504525281789</v>
+        <v>0.4616739866011528</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5559225975394744</v>
+        <v>0.5556674926208094</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5890156371236127</v>
+        <v>0.5888198148966381</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74623852133575</v>
+        <v>22.76645264330656</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29406113191247</v>
+        <v>12.29517394858069</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6740255086446632</v>
+        <v>0.673383608429558</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7506961663181104</v>
+        <v>0.7508290800637812</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.827532081539733</v>
+        <v>1.831352490248735</v>
       </c>
       <c r="D14" t="n">
-        <v>1.66442692177414</v>
+        <v>1.666409335600012</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>94.1628008016058</v>
+        <v>93.99678937053073</v>
       </c>
       <c r="D15" t="n">
-        <v>22.89926493004305</v>
+        <v>22.80897747747082</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -925,7 +925,7 @@
         <v>77.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>90.25999999999999</v>
+        <v>91.25999999999999</v>
       </c>
       <c r="H15" t="n">
         <v>110.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-86.02480107908279</v>
+        <v>-85.86187906500264</v>
       </c>
       <c r="D16" t="n">
-        <v>20.47195713110109</v>
+        <v>20.38336693616429</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.7376019773414</v>
+        <v>-102.2324940763249</v>
       </c>
       <c r="G16" t="n">
         <v>-84.23249407632485</v>
       </c>
       <c r="H16" t="n">
-        <v>-70.46683163887967</v>
+        <v>-70.26572375596102</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.60532520044909</v>
+        <v>-78.44663272592867</v>
       </c>
       <c r="D17" t="n">
-        <v>25.44454038663521</v>
+        <v>25.37424934572375</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.87736039420676</v>
+        <v>-93.41392685158225</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.57382219273629</v>
+        <v>-73.79009749652566</v>
       </c>
       <c r="H17" t="n">
-        <v>-60.41392685158225</v>
+        <v>-60.3175485570292</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
2M Rows upto !st Juli 25
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>536.8469228506967</v>
+        <v>532.2106212425854</v>
       </c>
       <c r="D2" t="n">
-        <v>129.7761258031</v>
+        <v>126.9954844019068</v>
       </c>
       <c r="E2" t="n">
         <v>386</v>
@@ -504,10 +504,10 @@
         <v>444</v>
       </c>
       <c r="G2" t="n">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H2" t="n">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36.37627465722989</v>
+        <v>36.51327065315416</v>
       </c>
       <c r="D3" t="n">
-        <v>6.672834355817785</v>
+        <v>6.585029651722805</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>31.37</v>
+        <v>31.67</v>
       </c>
       <c r="G3" t="n">
-        <v>36.49</v>
+        <v>36.67</v>
       </c>
       <c r="H3" t="n">
-        <v>40.78</v>
+        <v>40.85</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.922306955007867</v>
+        <v>2.051220549113259</v>
       </c>
       <c r="D4" t="n">
-        <v>2.60020301288987</v>
+        <v>2.674862232545927</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="G4" t="n">
-        <v>1.25</v>
+        <v>1.31</v>
       </c>
       <c r="H4" t="n">
-        <v>2.33</v>
+        <v>2.47</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.7852664719634</v>
+        <v>323.0362109370496</v>
       </c>
       <c r="D5" t="n">
-        <v>9.604742530486975</v>
+        <v>9.386588224888023</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.24</v>
+        <v>317.87</v>
       </c>
       <c r="G5" t="n">
-        <v>323.4</v>
+        <v>323.81</v>
       </c>
       <c r="H5" t="n">
-        <v>329.81</v>
+        <v>329.8</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22.16748994820075</v>
+        <v>22.58150089553854</v>
       </c>
       <c r="D6" t="n">
-        <v>2.911911700136196</v>
+        <v>3.266941800073979</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>20.31</v>
+        <v>20.42</v>
       </c>
       <c r="G6" t="n">
-        <v>22.08</v>
+        <v>22.28</v>
       </c>
       <c r="H6" t="n">
-        <v>23.97</v>
+        <v>24.51</v>
       </c>
       <c r="I6" t="n">
-        <v>43.95</v>
+        <v>45.32</v>
       </c>
     </row>
     <row r="7">
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.7367893705309</v>
+        <v>-76.69644376203388</v>
       </c>
       <c r="D7" t="n">
-        <v>22.80897747747082</v>
+        <v>22.87019877802588</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.415246339073944</v>
+        <v>7.415354158273629</v>
       </c>
       <c r="D8" t="n">
-        <v>7.114583036411164</v>
+        <v>7.104336290239358</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.322031633382492</v>
+        <v>9.321388809101659</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685562417434868</v>
+        <v>1.685678676124756</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8302641267222</v>
+        <v>867.8302548663114</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4616739866011528</v>
+        <v>0.4616805344479739</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5556674926208094</v>
+        <v>0.555527425568039</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5888198148966381</v>
+        <v>0.5888062665095325</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.76645264330656</v>
+        <v>22.76446408797683</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29517394858069</v>
+        <v>12.29682031832352</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.673383608429558</v>
+        <v>0.6736605395087145</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7508290800637812</v>
+        <v>0.7508222926507676</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.831352490248735</v>
+        <v>1.830988090064159</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666409335600012</v>
+        <v>1.666477230061925</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.99678937053073</v>
+        <v>93.95644376203364</v>
       </c>
       <c r="D15" t="n">
-        <v>22.80897747747082</v>
+        <v>22.87019877802589</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.86187906500264</v>
+        <v>-85.81856420269712</v>
       </c>
       <c r="D16" t="n">
-        <v>20.38336693616429</v>
+        <v>20.45211142633633</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.2324940763249</v>
+        <v>-102.3377954106368</v>
       </c>
       <c r="G16" t="n">
         <v>-84.23249407632485</v>
       </c>
       <c r="H16" t="n">
-        <v>-70.26572375596102</v>
+        <v>-70.07382219273629</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.44663272592867</v>
+        <v>-78.40321004442367</v>
       </c>
       <c r="D17" t="n">
-        <v>25.37424934572375</v>
+        <v>25.42481706855655</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.41392685158225</v>
+        <v>-93.49305820175223</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.79009749652566</v>
+        <v>-74.16954289279533</v>
       </c>
       <c r="H17" t="n">
-        <v>-60.3175485570292</v>
+        <v>-60.25410721860875</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
EDA from 4th Juli 25
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,25 +492,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>531.4469298571577</v>
+        <v>453.2580555555555</v>
       </c>
       <c r="D2" t="n">
-        <v>126.4953561647361</v>
+        <v>33.08451422318829</v>
       </c>
       <c r="E2" t="n">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="F2" t="n">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="G2" t="n">
-        <v>484</v>
+        <v>448</v>
       </c>
       <c r="H2" t="n">
-        <v>582</v>
+        <v>470</v>
       </c>
       <c r="I2" t="n">
-        <v>1993</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3">
@@ -525,25 +525,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36.4960841446557</v>
+        <v>35.78553560606061</v>
       </c>
       <c r="D3" t="n">
-        <v>6.562296531298776</v>
+        <v>4.437912724794431</v>
       </c>
       <c r="E3" t="n">
-        <v>13.96</v>
+        <v>22.73</v>
       </c>
       <c r="F3" t="n">
-        <v>31.68</v>
+        <v>32.36</v>
       </c>
       <c r="G3" t="n">
-        <v>36.62</v>
+        <v>35.78</v>
       </c>
       <c r="H3" t="n">
-        <v>40.82</v>
+        <v>39.07</v>
       </c>
       <c r="I3" t="n">
-        <v>60.19</v>
+        <v>50.85</v>
       </c>
     </row>
     <row r="4">
@@ -558,25 +558,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.053579207356649</v>
+        <v>1.750667171717172</v>
       </c>
       <c r="D4" t="n">
-        <v>2.66264873749152</v>
+        <v>1.101502338716308</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="F4" t="n">
-        <v>0.67</v>
+        <v>0.97</v>
       </c>
       <c r="G4" t="n">
-        <v>1.32</v>
+        <v>1.45</v>
       </c>
       <c r="H4" t="n">
-        <v>2.48</v>
+        <v>2.31</v>
       </c>
       <c r="I4" t="n">
-        <v>637.71</v>
+        <v>10.39</v>
       </c>
     </row>
     <row r="5">
@@ -591,25 +591,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>323.0613567390541</v>
+        <v>320.2051017676768</v>
       </c>
       <c r="D5" t="n">
-        <v>9.34682174835431</v>
+        <v>5.603780927290645</v>
       </c>
       <c r="E5" t="n">
-        <v>286.91</v>
+        <v>308.26</v>
       </c>
       <c r="F5" t="n">
-        <v>317.98</v>
+        <v>316.52</v>
       </c>
       <c r="G5" t="n">
-        <v>323.79</v>
+        <v>319.9</v>
       </c>
       <c r="H5" t="n">
-        <v>329.81</v>
+        <v>325.23</v>
       </c>
       <c r="I5" t="n">
-        <v>347.57</v>
+        <v>332.88</v>
       </c>
     </row>
     <row r="6">
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22.68327667206721</v>
+        <v>28.71858712121212</v>
       </c>
       <c r="D6" t="n">
-        <v>3.386244283997294</v>
+        <v>1.995589405843883</v>
       </c>
       <c r="E6" t="n">
-        <v>13.74</v>
+        <v>22.33</v>
       </c>
       <c r="F6" t="n">
-        <v>20.43</v>
+        <v>27.09</v>
       </c>
       <c r="G6" t="n">
-        <v>22.31</v>
+        <v>28.82</v>
       </c>
       <c r="H6" t="n">
-        <v>24.62</v>
+        <v>29.82</v>
       </c>
       <c r="I6" t="n">
-        <v>45.32</v>
+        <v>42.06</v>
       </c>
     </row>
     <row r="7">
@@ -657,25 +657,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.70777581243713</v>
+        <v>-70.23260101010101</v>
       </c>
       <c r="D7" t="n">
-        <v>22.90619956924442</v>
+        <v>19.48500092970017</v>
       </c>
       <c r="E7" t="n">
-        <v>-128</v>
+        <v>-121</v>
       </c>
       <c r="F7" t="n">
-        <v>-93</v>
+        <v>-86</v>
       </c>
       <c r="G7" t="n">
-        <v>-74</v>
+        <v>-69</v>
       </c>
       <c r="H7" t="n">
-        <v>-60</v>
+        <v>-50</v>
       </c>
       <c r="I7" t="n">
-        <v>-28</v>
+        <v>-35</v>
       </c>
     </row>
     <row r="8">
@@ -690,25 +690,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.400260037914754</v>
+        <v>9.808034157802984</v>
       </c>
       <c r="D8" t="n">
-        <v>7.114710859640799</v>
+        <v>3.354816805637959</v>
       </c>
       <c r="E8" t="n">
-        <v>-24.5</v>
+        <v>-19</v>
       </c>
       <c r="F8" t="n">
-        <v>7.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G8" t="n">
-        <v>9.5</v>
+        <v>10.2</v>
       </c>
       <c r="H8" t="n">
-        <v>11.2</v>
+        <v>11.8</v>
       </c>
       <c r="I8" t="n">
-        <v>25.2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.321231624477905</v>
+        <v>8.50320707070707</v>
       </c>
       <c r="D9" t="n">
-        <v>1.685729176198687</v>
+        <v>1.117449036735686</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -738,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="H9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" t="n">
         <v>11</v>
-      </c>
-      <c r="I9" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8302401514135</v>
+        <v>867.8014974747476</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4616751724702784</v>
+        <v>0.4588582799635839</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5555037193533202</v>
+        <v>0.2266959159595959</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5888227556170933</v>
+        <v>0.145131500830238</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -804,10 +804,10 @@
         <v>0.246784</v>
       </c>
       <c r="H11" t="n">
+        <v>0.452608</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.987136</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1.974272</v>
       </c>
     </row>
     <row r="12">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.76412939538525</v>
+        <v>22.74816919191919</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29661669839375</v>
+        <v>12.36859170704831</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6736447820206014</v>
+        <v>0.661060606060606</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7508014227362149</v>
+        <v>0.7506905444337185</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.831000688694997</v>
+        <v>1.830025252525252</v>
       </c>
       <c r="D14" t="n">
-        <v>1.666479761478036</v>
+        <v>1.690580924950423</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,25 +913,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.96777581243688</v>
+        <v>87.492601010101</v>
       </c>
       <c r="D15" t="n">
-        <v>22.90619956921905</v>
+        <v>19.48500092970293</v>
       </c>
       <c r="E15" t="n">
-        <v>45.26</v>
+        <v>52.26</v>
       </c>
       <c r="F15" t="n">
-        <v>77.25999999999999</v>
+        <v>67.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>91.25999999999999</v>
+        <v>86.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>110.26</v>
+        <v>103.26</v>
       </c>
       <c r="I15" t="n">
-        <v>145.26</v>
+        <v>138.26</v>
       </c>
     </row>
     <row r="16">
@@ -946,25 +946,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.82089427586178</v>
+        <v>-80.6473610253542</v>
       </c>
       <c r="D16" t="n">
-        <v>20.47873567228697</v>
+        <v>18.81304349493355</v>
       </c>
       <c r="E16" t="n">
-        <v>-141.2123840191425</v>
+        <v>-121.8240101588271</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.4139268515822</v>
+        <v>-96.96183611348224</v>
       </c>
       <c r="G16" t="n">
-        <v>-84.23249407632485</v>
+        <v>-80.45410721860875</v>
       </c>
       <c r="H16" t="n">
-        <v>-70.07382219273629</v>
+        <v>-61.33779541063677</v>
       </c>
       <c r="I16" t="n">
-        <v>-33.14609373817283</v>
+        <v>-42.95746206410165</v>
       </c>
     </row>
     <row r="17">
@@ -979,25 +979,25 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.42063423794706</v>
+        <v>-70.83932686755121</v>
       </c>
       <c r="D17" t="n">
-        <v>25.46633603633501</v>
+        <v>20.02536296935124</v>
       </c>
       <c r="E17" t="n">
-        <v>-146.5153820769794</v>
+        <v>-138.8714834061964</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.5149694202523</v>
+        <v>-86.5149694202523</v>
       </c>
       <c r="G17" t="n">
-        <v>-74.15142276599207</v>
+        <v>-69.49305820175223</v>
       </c>
       <c r="H17" t="n">
-        <v>-60.2376019773414</v>
+        <v>-50.33195619988427</v>
       </c>
       <c r="I17" t="n">
-        <v>-28.39612087980607</v>
+        <v>-35.57382219273629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
..... Checking stats per SF - EDA
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,25 +492,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>453.2580555555555</v>
+        <v>528.4482965277894</v>
       </c>
       <c r="D2" t="n">
-        <v>33.08451422318829</v>
+        <v>125.1079838022657</v>
       </c>
       <c r="E2" t="n">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="F2" t="n">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="G2" t="n">
-        <v>448</v>
+        <v>481</v>
       </c>
       <c r="H2" t="n">
-        <v>470</v>
+        <v>577</v>
       </c>
       <c r="I2" t="n">
-        <v>733</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="3">
@@ -525,25 +525,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>35.78553560606061</v>
+        <v>36.4645555298831</v>
       </c>
       <c r="D3" t="n">
-        <v>4.437912724794431</v>
+        <v>6.496280144131617</v>
       </c>
       <c r="E3" t="n">
-        <v>22.73</v>
+        <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.36</v>
+        <v>31.72</v>
       </c>
       <c r="G3" t="n">
-        <v>35.78</v>
+        <v>36.56</v>
       </c>
       <c r="H3" t="n">
-        <v>39.07</v>
+        <v>40.75</v>
       </c>
       <c r="I3" t="n">
-        <v>50.85</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="4">
@@ -558,25 +558,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.750667171717172</v>
+        <v>2.041738368201534</v>
       </c>
       <c r="D4" t="n">
-        <v>1.101502338716308</v>
+        <v>2.620411677440661</v>
       </c>
       <c r="E4" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.97</v>
+        <v>0.68</v>
       </c>
       <c r="G4" t="n">
-        <v>1.45</v>
+        <v>1.33</v>
       </c>
       <c r="H4" t="n">
-        <v>2.31</v>
+        <v>2.47</v>
       </c>
       <c r="I4" t="n">
-        <v>10.39</v>
+        <v>637.71</v>
       </c>
     </row>
     <row r="5">
@@ -591,25 +591,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>320.2051017676768</v>
+        <v>322.9604849232645</v>
       </c>
       <c r="D5" t="n">
-        <v>5.603780927290645</v>
+        <v>9.249139681571352</v>
       </c>
       <c r="E5" t="n">
-        <v>308.26</v>
+        <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>316.52</v>
+        <v>317.8</v>
       </c>
       <c r="G5" t="n">
-        <v>319.9</v>
+        <v>323.68</v>
       </c>
       <c r="H5" t="n">
-        <v>325.23</v>
+        <v>329.63</v>
       </c>
       <c r="I5" t="n">
-        <v>332.88</v>
+        <v>347.57</v>
       </c>
     </row>
     <row r="6">
@@ -624,25 +624,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>28.71858712121212</v>
+        <v>22.91639732837248</v>
       </c>
       <c r="D6" t="n">
-        <v>1.995589405843883</v>
+        <v>3.540605299298592</v>
       </c>
       <c r="E6" t="n">
-        <v>22.33</v>
+        <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>27.09</v>
+        <v>20.51</v>
       </c>
       <c r="G6" t="n">
-        <v>28.82</v>
+        <v>22.43</v>
       </c>
       <c r="H6" t="n">
-        <v>29.82</v>
+        <v>24.97</v>
       </c>
       <c r="I6" t="n">
-        <v>42.06</v>
+        <v>45.32</v>
       </c>
     </row>
     <row r="7">
@@ -657,25 +657,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-70.23260101010101</v>
+        <v>-76.46468263704121</v>
       </c>
       <c r="D7" t="n">
-        <v>19.48500092970017</v>
+        <v>22.82088736099912</v>
       </c>
       <c r="E7" t="n">
-        <v>-121</v>
+        <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-86</v>
+        <v>-93</v>
       </c>
       <c r="G7" t="n">
-        <v>-69</v>
+        <v>-73</v>
       </c>
       <c r="H7" t="n">
-        <v>-50</v>
+        <v>-59</v>
       </c>
       <c r="I7" t="n">
-        <v>-35</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="8">
@@ -690,25 +690,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9.808034157802984</v>
+        <v>7.490959019191643</v>
       </c>
       <c r="D8" t="n">
-        <v>3.354816805637959</v>
+        <v>7.024462455250215</v>
       </c>
       <c r="E8" t="n">
-        <v>-19</v>
+        <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>8.800000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="G8" t="n">
-        <v>10.2</v>
+        <v>9.5</v>
       </c>
       <c r="H8" t="n">
-        <v>11.8</v>
+        <v>11.2</v>
       </c>
       <c r="I8" t="n">
-        <v>17</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8.50320707070707</v>
+        <v>9.289980682151118</v>
       </c>
       <c r="D9" t="n">
-        <v>1.117449036735686</v>
+        <v>1.674951367790749</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -738,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I9" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8014974747476</v>
+        <v>867.8291466084195</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4588582799635839</v>
+        <v>0.461598568711231</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.2266959159595959</v>
+        <v>0.5429460117927014</v>
       </c>
       <c r="D11" t="n">
-        <v>0.145131500830238</v>
+        <v>0.581591921610971</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -804,10 +804,10 @@
         <v>0.246784</v>
       </c>
       <c r="H11" t="n">
-        <v>0.452608</v>
+        <v>0.987136</v>
       </c>
       <c r="I11" t="n">
-        <v>0.987136</v>
+        <v>1.974272</v>
       </c>
     </row>
     <row r="12">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74816919191919</v>
+        <v>22.76364242685538</v>
       </c>
       <c r="D12" t="n">
-        <v>12.36859170704831</v>
+        <v>12.2994770378161</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.661060606060606</v>
+        <v>0.6731634347182953</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7506905444337185</v>
+        <v>0.7508058844852884</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.830025252525252</v>
+        <v>1.830968107684502</v>
       </c>
       <c r="D14" t="n">
-        <v>1.690580924950423</v>
+        <v>1.6674234573675</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,25 +913,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>87.492601010101</v>
+        <v>93.72468263704091</v>
       </c>
       <c r="D15" t="n">
-        <v>19.48500092970293</v>
+        <v>22.82088736097611</v>
       </c>
       <c r="E15" t="n">
-        <v>52.26</v>
+        <v>45.26</v>
       </c>
       <c r="F15" t="n">
-        <v>67.25999999999999</v>
+        <v>76.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>86.25999999999999</v>
+        <v>90.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>103.26</v>
+        <v>110.26</v>
       </c>
       <c r="I15" t="n">
-        <v>138.26</v>
+        <v>145.26</v>
       </c>
     </row>
     <row r="16">
@@ -946,25 +946,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-80.6473610253542</v>
+        <v>-85.62665188965931</v>
       </c>
       <c r="D16" t="n">
-        <v>18.81304349493355</v>
+        <v>20.44308894419777</v>
       </c>
       <c r="E16" t="n">
-        <v>-121.8240101588271</v>
+        <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-96.96183611348224</v>
+        <v>-102.2108185264953</v>
       </c>
       <c r="G16" t="n">
-        <v>-80.45410721860875</v>
+        <v>-83.96183611348224</v>
       </c>
       <c r="H16" t="n">
-        <v>-61.33779541063677</v>
+        <v>-69.7376019773414</v>
       </c>
       <c r="I16" t="n">
-        <v>-42.95746206410165</v>
+        <v>-33.14609373817283</v>
       </c>
     </row>
     <row r="17">
@@ -979,25 +979,25 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-70.83932686755121</v>
+        <v>-78.13569287046764</v>
       </c>
       <c r="D17" t="n">
-        <v>20.02536296935124</v>
+        <v>25.32435936563775</v>
       </c>
       <c r="E17" t="n">
-        <v>-138.8714834061964</v>
+        <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-86.5149694202523</v>
+        <v>-93.3707776445072</v>
       </c>
       <c r="G17" t="n">
-        <v>-69.49305820175223</v>
+        <v>-73.3707776445072</v>
       </c>
       <c r="H17" t="n">
-        <v>-50.33195619988427</v>
+        <v>-59.34699179957641</v>
       </c>
       <c r="I17" t="n">
-        <v>-35.57382219273629</v>
+        <v>-28.39612087980607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Database with records up to 28th July
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>528.4482965277894</v>
+        <v>524.8646210551354</v>
       </c>
       <c r="D2" t="n">
-        <v>125.1079838022657</v>
+        <v>123.0273338117717</v>
       </c>
       <c r="E2" t="n">
         <v>381</v>
       </c>
       <c r="F2" t="n">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G2" t="n">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H2" t="n">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36.4645555298831</v>
+        <v>36.74248162610181</v>
       </c>
       <c r="D3" t="n">
-        <v>6.496280144131617</v>
+        <v>6.50264959182696</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>31.72</v>
+        <v>31.95</v>
       </c>
       <c r="G3" t="n">
-        <v>36.56</v>
+        <v>36.92</v>
       </c>
       <c r="H3" t="n">
-        <v>40.75</v>
+        <v>41.1</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.041738368201534</v>
+        <v>2.055739882564128</v>
       </c>
       <c r="D4" t="n">
-        <v>2.620411677440661</v>
+        <v>2.579004167187117</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="G4" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
       <c r="H4" t="n">
-        <v>2.47</v>
+        <v>2.51</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.9604849232645</v>
+        <v>322.7356937847636</v>
       </c>
       <c r="D5" t="n">
-        <v>9.249139681571352</v>
+        <v>9.094335613087898</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.8</v>
+        <v>317.69</v>
       </c>
       <c r="G5" t="n">
-        <v>323.68</v>
+        <v>323.21</v>
       </c>
       <c r="H5" t="n">
-        <v>329.63</v>
+        <v>329.32</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22.91639732837248</v>
+        <v>23.17586993857387</v>
       </c>
       <c r="D6" t="n">
-        <v>3.540605299298592</v>
+        <v>3.641445351245375</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>20.51</v>
+        <v>20.63</v>
       </c>
       <c r="G6" t="n">
-        <v>22.43</v>
+        <v>22.62</v>
       </c>
       <c r="H6" t="n">
-        <v>24.97</v>
+        <v>25.45</v>
       </c>
       <c r="I6" t="n">
         <v>45.32</v>
@@ -657,22 +657,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.46468263704121</v>
+        <v>-76.09269390708312</v>
       </c>
       <c r="D7" t="n">
-        <v>22.82088736099912</v>
+        <v>22.57171239534686</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-93</v>
+        <v>-92</v>
       </c>
       <c r="G7" t="n">
-        <v>-73</v>
+        <v>-72</v>
       </c>
       <c r="H7" t="n">
-        <v>-59</v>
+        <v>-58</v>
       </c>
       <c r="I7" t="n">
         <v>-28</v>
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.490959019191643</v>
+        <v>7.625479137831975</v>
       </c>
       <c r="D8" t="n">
-        <v>7.024462455250215</v>
+        <v>6.888120590547293</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>7.8</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
         <v>9.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.289980682151118</v>
+        <v>9.248521444527144</v>
       </c>
       <c r="D9" t="n">
-        <v>1.674951367790749</v>
+        <v>1.659694962714828</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8291466084195</v>
+        <v>867.8277592894087</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461598568711231</v>
+        <v>0.4614728077845632</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5429460117927014</v>
+        <v>0.5263110209265871</v>
       </c>
       <c r="D11" t="n">
-        <v>0.581591921610971</v>
+        <v>0.5714624939927891</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.76364242685538</v>
+        <v>22.75806666374785</v>
       </c>
       <c r="D12" t="n">
-        <v>12.2994770378161</v>
+        <v>12.29785793976647</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6731634347182953</v>
+        <v>0.6728080750816856</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7508058844852884</v>
+        <v>0.7505323477745689</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.830968107684502</v>
+        <v>1.830958331433843</v>
       </c>
       <c r="D14" t="n">
-        <v>1.6674234573675</v>
+        <v>1.667744089936605</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,22 +913,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.72468263704091</v>
+        <v>93.35269390708277</v>
       </c>
       <c r="D15" t="n">
-        <v>22.82088736097611</v>
+        <v>22.57171239534685</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
       </c>
       <c r="F15" t="n">
-        <v>76.25999999999999</v>
+        <v>75.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>90.25999999999999</v>
+        <v>89.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>110.26</v>
+        <v>109.26</v>
       </c>
       <c r="I15" t="n">
         <v>145.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.62665188965931</v>
+        <v>-85.3279545708132</v>
       </c>
       <c r="D16" t="n">
-        <v>20.44308894419777</v>
+        <v>20.25890582329711</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-102.2108185264953</v>
+        <v>-101.6389203414338</v>
       </c>
       <c r="G16" t="n">
-        <v>-83.96183611348224</v>
+        <v>-83.33195619988427</v>
       </c>
       <c r="H16" t="n">
-        <v>-69.7376019773414</v>
+        <v>-69.6389203414338</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-78.13569287046764</v>
+        <v>-77.70247543298126</v>
       </c>
       <c r="D17" t="n">
-        <v>25.32435936563775</v>
+        <v>25.00224010122128</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-93.3707776445072</v>
+        <v>-92.57382219273629</v>
       </c>
       <c r="G17" t="n">
-        <v>-73.3707776445072</v>
+        <v>-72.46183611348224</v>
       </c>
       <c r="H17" t="n">
-        <v>-59.34699179957641</v>
+        <v>-58.75746206410165</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
More data + the necessary cleaning procedures.
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>524.8646210551354</v>
+        <v>523.5861948266684</v>
       </c>
       <c r="D2" t="n">
-        <v>123.0273338117717</v>
+        <v>122.0436772156639</v>
       </c>
       <c r="E2" t="n">
         <v>381</v>
@@ -504,10 +504,10 @@
         <v>442</v>
       </c>
       <c r="G2" t="n">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H2" t="n">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36.74248162610181</v>
+        <v>36.84388973146382</v>
       </c>
       <c r="D3" t="n">
-        <v>6.50264959182696</v>
+        <v>6.489012600754923</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>31.95</v>
+        <v>32.05</v>
       </c>
       <c r="G3" t="n">
-        <v>36.92</v>
+        <v>37.09</v>
       </c>
       <c r="H3" t="n">
-        <v>41.1</v>
+        <v>41.22</v>
       </c>
       <c r="I3" t="n">
         <v>60.19</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.055739882564128</v>
+        <v>2.083656679063995</v>
       </c>
       <c r="D4" t="n">
-        <v>2.579004167187117</v>
+        <v>2.57745453201037</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="G4" t="n">
-        <v>1.36</v>
+        <v>1.38</v>
       </c>
       <c r="H4" t="n">
-        <v>2.51</v>
+        <v>2.56</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.7356937847636</v>
+        <v>322.7980935511237</v>
       </c>
       <c r="D5" t="n">
-        <v>9.094335613087898</v>
+        <v>9.021253159600393</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.69</v>
+        <v>317.87</v>
       </c>
       <c r="G5" t="n">
-        <v>323.21</v>
+        <v>323.26</v>
       </c>
       <c r="H5" t="n">
-        <v>329.32</v>
+        <v>329.3</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23.17586993857387</v>
+        <v>23.26879912621351</v>
       </c>
       <c r="D6" t="n">
-        <v>3.641445351245375</v>
+        <v>3.665981481259716</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>20.63</v>
+        <v>20.68</v>
       </c>
       <c r="G6" t="n">
-        <v>22.62</v>
+        <v>22.71</v>
       </c>
       <c r="H6" t="n">
-        <v>25.45</v>
+        <v>25.66</v>
       </c>
       <c r="I6" t="n">
         <v>45.32</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-76.09269390708312</v>
+        <v>-75.98254104315876</v>
       </c>
       <c r="D7" t="n">
-        <v>22.57171239534686</v>
+        <v>22.50803120461898</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.625479137831975</v>
+        <v>7.664853278133452</v>
       </c>
       <c r="D8" t="n">
-        <v>6.888120590547293</v>
+        <v>6.848737824671677</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.248521444527144</v>
+        <v>9.231929931115822</v>
       </c>
       <c r="D9" t="n">
-        <v>1.659694962714828</v>
+        <v>1.653348633136656</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8277592894087</v>
+        <v>867.8271661262509</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4614728077845632</v>
+        <v>0.4614243558677465</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5263110209265871</v>
+        <v>0.5196793326382828</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5714624939927891</v>
+        <v>0.5672473917880538</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.75806666374785</v>
+        <v>22.75735960754645</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29785793976647</v>
+        <v>12.29755897919453</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6728080750816856</v>
+        <v>0.6726814157495205</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7505323477745689</v>
+        <v>0.7504897251850829</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.830958331433843</v>
+        <v>1.830998939768056</v>
       </c>
       <c r="D14" t="n">
-        <v>1.667744089936605</v>
+        <v>1.667848296399615</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.35269390708277</v>
+        <v>93.2425410431584</v>
       </c>
       <c r="D15" t="n">
-        <v>22.57171239534685</v>
+        <v>22.50803120461897</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.3279545708132</v>
+        <v>-85.23947718154869</v>
       </c>
       <c r="D16" t="n">
-        <v>20.25890582329711</v>
+        <v>20.2133753453302</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.6389203414338</v>
+        <v>-101.5175485570292</v>
       </c>
       <c r="G16" t="n">
-        <v>-83.33195619988427</v>
+        <v>-83.14699179957641</v>
       </c>
       <c r="H16" t="n">
-        <v>-69.6389203414338</v>
+        <v>-69.45410721860875</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.70247543298126</v>
+        <v>-77.5746239034152</v>
       </c>
       <c r="D17" t="n">
-        <v>25.00224010122128</v>
+        <v>24.91663364700802</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.57382219273629</v>
+        <v>-92.49305820175223</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.46183611348224</v>
+        <v>-72.41392685158225</v>
       </c>
       <c r="H17" t="n">
-        <v>-58.75746206410165</v>
+        <v>-58.53779541063678</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
Data Querrying + Relevant processes upto ENV fLDPLM fitting.
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>521.249714162698</v>
+        <v>517.416566736907</v>
       </c>
       <c r="D2" t="n">
-        <v>120.3459446352726</v>
+        <v>118.2430090347994</v>
       </c>
       <c r="E2" t="n">
         <v>381</v>
       </c>
       <c r="F2" t="n">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G2" t="n">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H2" t="n">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,25 +525,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36.89600256215319</v>
+        <v>37.08015121039799</v>
       </c>
       <c r="D3" t="n">
-        <v>6.428824730282332</v>
+        <v>6.48922326979137</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.21</v>
+        <v>32.36</v>
       </c>
       <c r="G3" t="n">
-        <v>37.12</v>
+        <v>37.22</v>
       </c>
       <c r="H3" t="n">
-        <v>41.23</v>
+        <v>41.42</v>
       </c>
       <c r="I3" t="n">
-        <v>60.19</v>
+        <v>62.81</v>
       </c>
     </row>
     <row r="4">
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.147963609457676</v>
+        <v>2.103507656356632</v>
       </c>
       <c r="D4" t="n">
-        <v>2.620564809005651</v>
+        <v>2.580611799609351</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="G4" t="n">
-        <v>1.4</v>
+        <v>1.36</v>
       </c>
       <c r="H4" t="n">
-        <v>2.63</v>
+        <v>2.58</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.8131976485485</v>
+        <v>322.5873181168558</v>
       </c>
       <c r="D5" t="n">
-        <v>8.880905108495368</v>
+        <v>8.773077343613297</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.95</v>
+        <v>317.43</v>
       </c>
       <c r="G5" t="n">
-        <v>323.3</v>
+        <v>323.09</v>
       </c>
       <c r="H5" t="n">
-        <v>329.07</v>
+        <v>328.75</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23.51716640095875</v>
+        <v>23.68275723078164</v>
       </c>
       <c r="D6" t="n">
-        <v>3.819687077437876</v>
+        <v>3.79232396646391</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>20.78</v>
+        <v>20.91</v>
       </c>
       <c r="G6" t="n">
-        <v>22.87</v>
+        <v>23.16</v>
       </c>
       <c r="H6" t="n">
-        <v>26.16</v>
+        <v>26.38</v>
       </c>
       <c r="I6" t="n">
         <v>46.29</v>
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-75.86856272783288</v>
+        <v>-75.55727063374835</v>
       </c>
       <c r="D7" t="n">
-        <v>22.38376199587726</v>
+        <v>22.23745506296449</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-92</v>
+        <v>-91</v>
       </c>
       <c r="G7" t="n">
         <v>-72</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.729336528910759</v>
+        <v>7.828773339471671</v>
       </c>
       <c r="D8" t="n">
-        <v>6.770735794126646</v>
+        <v>6.672697927244556</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.202788534639922</v>
+        <v>9.162045139899666</v>
       </c>
       <c r="D9" t="n">
-        <v>1.641612831792344</v>
+        <v>1.6243388762162</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8260909916117</v>
+        <v>867.8246188992435</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4613338988877554</v>
+        <v>0.4612275166605061</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.507986873503539</v>
+        <v>0.4917044040828045</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5595190944562856</v>
+        <v>0.5482100045929824</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.7550558664663</v>
+        <v>22.74950993487495</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29785951693799</v>
+        <v>12.29619773727692</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6724139246203173</v>
+        <v>0.6722120196034036</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7503883360236313</v>
+        <v>0.7501695231887071</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.830967812473779</v>
+        <v>1.830738753459606</v>
       </c>
       <c r="D14" t="n">
-        <v>1.668247588202604</v>
+        <v>1.668290349302445</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>93.12856272783289</v>
+        <v>92.81727063374788</v>
       </c>
       <c r="D15" t="n">
-        <v>22.38376199587726</v>
+        <v>22.2374550630588</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -928,7 +928,7 @@
         <v>89.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>109.26</v>
+        <v>108.26</v>
       </c>
       <c r="I15" t="n">
         <v>145.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-85.15643207069809</v>
+        <v>-84.9017073378634</v>
       </c>
       <c r="D16" t="n">
-        <v>20.11903951893733</v>
+        <v>20.02160869245486</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-101.4139268515822</v>
+        <v>-100.9574620641016</v>
       </c>
       <c r="G16" t="n">
-        <v>-82.8707776445072</v>
+        <v>-82.46683163887967</v>
       </c>
       <c r="H16" t="n">
-        <v>-69.45410721860875</v>
+        <v>-69.0778545523916</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-77.42709554178732</v>
+        <v>-77.07293399839182</v>
       </c>
       <c r="D17" t="n">
-        <v>24.74555802338096</v>
+        <v>24.544925109817</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-92.39612087980606</v>
+        <v>-91.6389203414338</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.3175485570292</v>
+        <v>-72.2376019773414</v>
       </c>
       <c r="H17" t="n">
-        <v>-58.5149694202523</v>
+        <v>-58.3175485570292</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
EDA and results  up to 29th Sept 2025
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>516.1387240229359</v>
+        <v>516.0566398604303</v>
       </c>
       <c r="D2" t="n">
-        <v>117.0474683613837</v>
+        <v>117.0786055004925</v>
       </c>
       <c r="E2" t="n">
         <v>381</v>
@@ -504,7 +504,7 @@
         <v>441</v>
       </c>
       <c r="G2" t="n">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H2" t="n">
         <v>550</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.35960358653833</v>
+        <v>37.3764503358322</v>
       </c>
       <c r="D3" t="n">
-        <v>6.522499419468365</v>
+        <v>6.484512362060585</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.63</v>
+        <v>32.71</v>
       </c>
       <c r="G3" t="n">
-        <v>37.58</v>
+        <v>37.59</v>
       </c>
       <c r="H3" t="n">
-        <v>41.76</v>
+        <v>41.75</v>
       </c>
       <c r="I3" t="n">
         <v>62.81</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.068631474455214</v>
+        <v>2.049962455625566</v>
       </c>
       <c r="D4" t="n">
-        <v>2.543118841843982</v>
+        <v>2.527692175702072</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="G4" t="n">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
       <c r="H4" t="n">
-        <v>2.54</v>
+        <v>2.52</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.5380583381891</v>
+        <v>322.6127146072568</v>
       </c>
       <c r="D5" t="n">
-        <v>8.620341419966229</v>
+        <v>8.557186073890973</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.53</v>
+        <v>317.69</v>
       </c>
       <c r="G5" t="n">
-        <v>323</v>
+        <v>323.15</v>
       </c>
       <c r="H5" t="n">
-        <v>328.48</v>
+        <v>328.38</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23.74778191128934</v>
+        <v>23.74303325768589</v>
       </c>
       <c r="D6" t="n">
-        <v>3.727612114733773</v>
+        <v>3.700514144655235</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>21.03</v>
+        <v>21.06</v>
       </c>
       <c r="G6" t="n">
         <v>23.38</v>
       </c>
       <c r="H6" t="n">
-        <v>26.33</v>
+        <v>26.29</v>
       </c>
       <c r="I6" t="n">
         <v>46.29</v>
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-75.29857362216457</v>
+        <v>-75.18715237466306</v>
       </c>
       <c r="D7" t="n">
-        <v>22.13776827725802</v>
+        <v>22.09337141334001</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -669,10 +669,10 @@
         <v>-91</v>
       </c>
       <c r="G7" t="n">
-        <v>-72</v>
+        <v>-71</v>
       </c>
       <c r="H7" t="n">
-        <v>-58</v>
+        <v>-57</v>
       </c>
       <c r="I7" t="n">
         <v>-28</v>
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.915268512468279</v>
+        <v>7.954853436707918</v>
       </c>
       <c r="D8" t="n">
-        <v>6.578895236994517</v>
+        <v>6.536677735626419</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.129496127047274</v>
+        <v>9.117618181906218</v>
       </c>
       <c r="D9" t="n">
-        <v>1.609415671911554</v>
+        <v>1.603902592242946</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8234552698152</v>
+        <v>867.8230302332785</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4611224540649217</v>
+        <v>0.4610855562334063</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4786169616265453</v>
+        <v>0.4738713281166023</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5385496123288287</v>
+        <v>0.5349304607510091</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74704427560315</v>
+        <v>22.74796290109255</v>
       </c>
       <c r="D12" t="n">
-        <v>12.2969273372467</v>
+        <v>12.29667879762277</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6718397142309422</v>
+        <v>0.6717072224127997</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7500267175241916</v>
+        <v>0.7500108620957644</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.830858351095834</v>
+        <v>1.831115496254315</v>
       </c>
       <c r="D14" t="n">
-        <v>1.668980905261562</v>
+        <v>1.669134238883229</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,19 +913,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>92.55857362216403</v>
+        <v>92.44715237466252</v>
       </c>
       <c r="D15" t="n">
-        <v>22.137768277258</v>
+        <v>22.09337141331377</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
       </c>
       <c r="F15" t="n">
-        <v>75.25999999999999</v>
+        <v>74.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>89.25999999999999</v>
+        <v>88.25999999999999</v>
       </c>
       <c r="H15" t="n">
         <v>108.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-84.69060323874157</v>
+        <v>-84.60145774217064</v>
       </c>
       <c r="D16" t="n">
-        <v>19.96737969448842</v>
+        <v>19.94693935633377</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-100.6389203414338</v>
+        <v>-100.5961208798061</v>
       </c>
       <c r="G16" t="n">
-        <v>-82.26572375596102</v>
+        <v>-82.23249407632485</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.7376019773414</v>
+        <v>-68.59612087980607</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-76.77533472627326</v>
+        <v>-76.64660430546279</v>
       </c>
       <c r="D17" t="n">
-        <v>24.38924546584868</v>
+        <v>24.31944969061291</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-91.39612087980606</v>
+        <v>-91.34699179957641</v>
       </c>
       <c r="G17" t="n">
-        <v>-72.18978441047734</v>
+        <v>-71.41392685158225</v>
       </c>
       <c r="H17" t="n">
-        <v>-58.22214159641585</v>
+        <v>-57.75746206410165</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
EDA up to 09-10-2025
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>516.0566398604303</v>
+        <v>519.0470293638949</v>
       </c>
       <c r="D2" t="n">
-        <v>117.0786055004925</v>
+        <v>121.0308980644043</v>
       </c>
       <c r="E2" t="n">
         <v>381</v>
@@ -504,10 +504,10 @@
         <v>441</v>
       </c>
       <c r="G2" t="n">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H2" t="n">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.3764503358322</v>
+        <v>37.48204644382814</v>
       </c>
       <c r="D3" t="n">
-        <v>6.484512362060585</v>
+        <v>6.462295981724989</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.71</v>
+        <v>32.87</v>
       </c>
       <c r="G3" t="n">
-        <v>37.59</v>
+        <v>37.68</v>
       </c>
       <c r="H3" t="n">
-        <v>41.75</v>
+        <v>41.87</v>
       </c>
       <c r="I3" t="n">
         <v>62.81</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.049962455625566</v>
+        <v>2.034764764627279</v>
       </c>
       <c r="D4" t="n">
-        <v>2.527692175702072</v>
+        <v>2.498994627991414</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -573,7 +573,7 @@
         <v>1.32</v>
       </c>
       <c r="H4" t="n">
-        <v>2.52</v>
+        <v>2.51</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.6127146072568</v>
+        <v>322.7068557850753</v>
       </c>
       <c r="D5" t="n">
-        <v>8.557186073890973</v>
+        <v>8.550966776585174</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.69</v>
+        <v>317.77</v>
       </c>
       <c r="G5" t="n">
-        <v>323.15</v>
+        <v>323.29</v>
       </c>
       <c r="H5" t="n">
-        <v>328.38</v>
+        <v>328.53</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23.74303325768589</v>
+        <v>23.71782131545305</v>
       </c>
       <c r="D6" t="n">
-        <v>3.700514144655235</v>
+        <v>3.660608368792933</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>21.06</v>
+        <v>21.11</v>
       </c>
       <c r="G6" t="n">
-        <v>23.38</v>
+        <v>23.32</v>
       </c>
       <c r="H6" t="n">
-        <v>26.29</v>
+        <v>26.21</v>
       </c>
       <c r="I6" t="n">
         <v>46.29</v>
@@ -657,19 +657,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-75.18715237466306</v>
+        <v>-75.02723897846421</v>
       </c>
       <c r="D7" t="n">
-        <v>22.09337141334001</v>
+        <v>22.03234664286968</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-91</v>
+        <v>-90</v>
       </c>
       <c r="G7" t="n">
-        <v>-71</v>
+        <v>-70</v>
       </c>
       <c r="H7" t="n">
         <v>-57</v>
@@ -690,22 +690,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.954853436707918</v>
+        <v>8.003956186816254</v>
       </c>
       <c r="D8" t="n">
-        <v>6.536677735626419</v>
+        <v>6.482616637954716</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="G8" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>11.2</v>
+        <v>11.5</v>
       </c>
       <c r="I8" t="n">
         <v>25.2</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.117618181906218</v>
+        <v>9.099572884200908</v>
       </c>
       <c r="D9" t="n">
-        <v>1.603902592242946</v>
+        <v>1.594939389211567</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8230302332785</v>
+        <v>867.8223341045298</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4610855562334063</v>
+        <v>0.461020912626382</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4738713281166023</v>
+        <v>0.466567421990915</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5349304607510091</v>
+        <v>0.5292003112480498</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.74796290109255</v>
+        <v>22.75176248067642</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29667879762277</v>
+        <v>12.29563296379348</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6717072224127997</v>
+        <v>0.6714732404741105</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7500108620957644</v>
+        <v>0.7500371934682567</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.831115496254315</v>
+        <v>1.831828711275575</v>
       </c>
       <c r="D14" t="n">
-        <v>1.669134238883229</v>
+        <v>1.669297308196148</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>92.44715237466252</v>
+        <v>92.28723897846365</v>
       </c>
       <c r="D15" t="n">
-        <v>22.09337141331377</v>
+        <v>22.03234664286967</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -925,10 +925,10 @@
         <v>74.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>88.25999999999999</v>
+        <v>87.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>108.26</v>
+        <v>107.26</v>
       </c>
       <c r="I15" t="n">
         <v>145.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-84.60145774217064</v>
+        <v>-84.46743065575667</v>
       </c>
       <c r="D16" t="n">
-        <v>19.94693935633377</v>
+        <v>19.90755133025647</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-100.5961208798061</v>
+        <v>-100.265723755961</v>
       </c>
       <c r="G16" t="n">
-        <v>-82.23249407632485</v>
+        <v>-82.0778545523916</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.59612087980607</v>
+        <v>-68.41392685158225</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-76.64660430546279</v>
+        <v>-76.46347446894042</v>
       </c>
       <c r="D17" t="n">
-        <v>24.31944969061291</v>
+        <v>24.22605095149054</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-91.34699179957641</v>
+        <v>-90.57382219273629</v>
       </c>
       <c r="G17" t="n">
-        <v>-71.41392685158225</v>
+        <v>-70.66683163887967</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.75746206410165</v>
+        <v>-57.5149694202523</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>

<commit_message>
Aligning the dataspan: 1 year
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -492,22 +492,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>519.0470293638949</v>
+        <v>517.6224248938721</v>
       </c>
       <c r="D2" t="n">
-        <v>121.0308980644043</v>
+        <v>118.5645605878984</v>
       </c>
       <c r="E2" t="n">
         <v>381</v>
       </c>
       <c r="F2" t="n">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G2" t="n">
         <v>473</v>
       </c>
       <c r="H2" t="n">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I2" t="n">
         <v>1993</v>
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37.48204644382814</v>
+        <v>37.34575783424336</v>
       </c>
       <c r="D3" t="n">
-        <v>6.462295981724989</v>
+        <v>6.482859032778124</v>
       </c>
       <c r="E3" t="n">
         <v>13.96</v>
       </c>
       <c r="F3" t="n">
-        <v>32.87</v>
+        <v>32.67</v>
       </c>
       <c r="G3" t="n">
-        <v>37.68</v>
+        <v>37.55</v>
       </c>
       <c r="H3" t="n">
-        <v>41.87</v>
+        <v>41.73</v>
       </c>
       <c r="I3" t="n">
         <v>62.81</v>
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.034764764627279</v>
+        <v>2.064765594994014</v>
       </c>
       <c r="D4" t="n">
-        <v>2.498994627991414</v>
+        <v>2.53455505977305</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="G4" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="H4" t="n">
-        <v>2.51</v>
+        <v>2.54</v>
       </c>
       <c r="I4" t="n">
         <v>637.71</v>
@@ -591,22 +591,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>322.7068557850753</v>
+        <v>322.6969035089136</v>
       </c>
       <c r="D5" t="n">
-        <v>8.550966776585174</v>
+        <v>8.494172126422965</v>
       </c>
       <c r="E5" t="n">
         <v>286.91</v>
       </c>
       <c r="F5" t="n">
-        <v>317.77</v>
+        <v>317.8</v>
       </c>
       <c r="G5" t="n">
-        <v>323.29</v>
+        <v>323.21</v>
       </c>
       <c r="H5" t="n">
-        <v>328.53</v>
+        <v>328.4</v>
       </c>
       <c r="I5" t="n">
         <v>347.57</v>
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23.71782131545305</v>
+        <v>23.74074421510393</v>
       </c>
       <c r="D6" t="n">
-        <v>3.660608368792933</v>
+        <v>3.711613999081814</v>
       </c>
       <c r="E6" t="n">
         <v>13.74</v>
       </c>
       <c r="F6" t="n">
-        <v>21.11</v>
+        <v>21.05</v>
       </c>
       <c r="G6" t="n">
-        <v>23.32</v>
+        <v>23.36</v>
       </c>
       <c r="H6" t="n">
-        <v>26.21</v>
+        <v>26.31</v>
       </c>
       <c r="I6" t="n">
         <v>46.29</v>
@@ -657,19 +657,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-75.02723897846421</v>
+        <v>-75.11641989524432</v>
       </c>
       <c r="D7" t="n">
-        <v>22.03234664286968</v>
+        <v>22.05405367114712</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-90</v>
+        <v>-91</v>
       </c>
       <c r="G7" t="n">
-        <v>-70</v>
+        <v>-71</v>
       </c>
       <c r="H7" t="n">
         <v>-57</v>
@@ -690,22 +690,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>8.003956186816254</v>
+        <v>7.9713349218551</v>
       </c>
       <c r="D8" t="n">
-        <v>6.482616637954716</v>
+        <v>6.526893324470904</v>
       </c>
       <c r="E8" t="n">
         <v>-24.5</v>
       </c>
       <c r="F8" t="n">
-        <v>8.199999999999999</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>11.5</v>
+        <v>11.2</v>
       </c>
       <c r="I8" t="n">
         <v>25.2</v>
@@ -723,10 +723,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.099572884200908</v>
+        <v>9.112710158057105</v>
       </c>
       <c r="D9" t="n">
-        <v>1.594939389211567</v>
+        <v>1.601501744710999</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>867.8223341045298</v>
+        <v>867.8228457262176</v>
       </c>
       <c r="D10" t="n">
-        <v>0.461020912626382</v>
+        <v>0.4610641877304697</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.466567421990915</v>
+        <v>0.4718851948034393</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5292003112480498</v>
+        <v>0.5333773730009826</v>
       </c>
       <c r="E11" t="n">
         <v>0.071936</v>
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22.75176248067642</v>
+        <v>22.74755277862356</v>
       </c>
       <c r="D12" t="n">
-        <v>12.29563296379348</v>
+        <v>12.2962608807795</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -851,10 +851,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>0.6714732404741105</v>
+        <v>0.6716223689530927</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7500371934682567</v>
+        <v>0.7499756835717255</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1.831828711275575</v>
+        <v>1.831174106852896</v>
       </c>
       <c r="D14" t="n">
-        <v>1.669297308196148</v>
+        <v>1.669175369014386</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>92.28723897846365</v>
+        <v>92.3764198952438</v>
       </c>
       <c r="D15" t="n">
-        <v>22.03234664286967</v>
+        <v>22.05405367114713</v>
       </c>
       <c r="E15" t="n">
         <v>45.26</v>
@@ -925,10 +925,10 @@
         <v>74.25999999999999</v>
       </c>
       <c r="G15" t="n">
-        <v>87.25999999999999</v>
+        <v>88.25999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>107.26</v>
+        <v>108.26</v>
       </c>
       <c r="I15" t="n">
         <v>145.26</v>
@@ -946,22 +946,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-84.46743065575667</v>
+        <v>-84.54313662807775</v>
       </c>
       <c r="D16" t="n">
-        <v>19.90755133025647</v>
+        <v>19.91707498201135</v>
       </c>
       <c r="E16" t="n">
         <v>-141.2123840191425</v>
       </c>
       <c r="F16" t="n">
-        <v>-100.265723755961</v>
+        <v>-100.4668316388797</v>
       </c>
       <c r="G16" t="n">
-        <v>-82.0778545523916</v>
+        <v>-82.21081852649533</v>
       </c>
       <c r="H16" t="n">
-        <v>-68.41392685158225</v>
+        <v>-68.5175485570292</v>
       </c>
       <c r="I16" t="n">
         <v>-33.14609373817283</v>
@@ -979,22 +979,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-76.46347446894042</v>
+        <v>-76.57180170622264</v>
       </c>
       <c r="D17" t="n">
-        <v>24.22605095149054</v>
+        <v>24.27898143112502</v>
       </c>
       <c r="E17" t="n">
         <v>-146.5153820769794</v>
       </c>
       <c r="F17" t="n">
-        <v>-90.57382219273629</v>
+        <v>-91.2778545523916</v>
       </c>
       <c r="G17" t="n">
-        <v>-70.66683163887967</v>
+        <v>-70.79009749652566</v>
       </c>
       <c r="H17" t="n">
-        <v>-57.5149694202523</v>
+        <v>-57.75746206410165</v>
       </c>
       <c r="I17" t="n">
         <v>-28.39612087980607</v>

</xml_diff>